<commit_message>
add como to macro and change in macro
</commit_message>
<xml_diff>
--- a/database/macro/commodity.xlsx
+++ b/database/macro/commodity.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="کرک اسپرد نفت" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
   <si>
     <t>فرآورده</t>
   </si>
@@ -116,15 +116,6 @@
     <t>Change</t>
   </si>
   <si>
-    <t>تاریخ</t>
-  </si>
-  <si>
-    <t>اوره</t>
-  </si>
-  <si>
-    <t>متانول</t>
-  </si>
-  <si>
     <t>کائوچو</t>
   </si>
   <si>
@@ -198,6 +189,12 @@
   </si>
   <si>
     <t>1401/7/30</t>
+  </si>
+  <si>
+    <t>urea</t>
+  </si>
+  <si>
+    <t>methanol</t>
   </si>
 </sst>
 </file>
@@ -314,3050 +311,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="95000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:effectLst>
-                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-                    <a:prstClr val="black">
-                      <a:alpha val="40000"/>
-                    </a:prstClr>
-                  </a:outerShdw>
-                </a:effectLst>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="B Nazanin" panose="00000400000000000000" pitchFamily="2" charset="-78"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="fa-IR">
-                <a:cs typeface="B Nazanin" panose="00000400000000000000" pitchFamily="2" charset="-78"/>
-              </a:rPr>
-              <a:t>نرخ اوره</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US">
-              <a:cs typeface="B Nazanin" panose="00000400000000000000" pitchFamily="2" charset="-78"/>
-            </a:endParaRPr>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:effectLst>
-                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-                  <a:prstClr val="black">
-                    <a:alpha val="40000"/>
-                  </a:prstClr>
-                </a:outerShdw>
-              </a:effectLst>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="B Nazanin" panose="00000400000000000000" pitchFamily="2" charset="-78"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="34925" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'اوره بلندمدت'!$A$2:$A$361</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="360"/>
-                <c:pt idx="0">
-                  <c:v>33878</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>33909</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>33939</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>33970</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>34001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>34029</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>34060</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>34090</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>34121</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>34151</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>34182</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>34213</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>34243</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>34274</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>34304</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>34335</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>34366</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>34394</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>34425</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>34455</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>34486</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>34516</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>34547</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>34578</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>34608</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>34639</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>34669</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>34700</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>34731</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>34759</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>34790</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>34820</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>34851</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>34881</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>34912</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>34943</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>34973</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>35004</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>35034</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>35065</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>35096</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>35125</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>35156</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>35186</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>35217</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>35247</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>35278</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>35309</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>35339</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>35370</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>35400</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>35431</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>35462</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>35490</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>35521</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>35551</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>35582</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>35612</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>35643</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>35674</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>35704</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>35735</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>35765</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>35796</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>35827</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>35855</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>35886</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>35916</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>35947</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>35977</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>36008</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>36039</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>36069</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>36100</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>36130</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>36161</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>36192</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>36220</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>36251</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>36281</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>36312</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>36342</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>36373</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>36404</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>36434</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>36465</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>36495</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>36526</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>36557</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>36586</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>36617</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>36647</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>36678</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>36708</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>36739</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>36770</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>36800</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>36831</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>36861</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>36892</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>36923</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>36951</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>36982</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>37012</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>37043</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>37073</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>37104</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>37135</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>37165</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>37196</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>37226</c:v>
-                </c:pt>
-                <c:pt idx="111">
-                  <c:v>37257</c:v>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v>37288</c:v>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v>37316</c:v>
-                </c:pt>
-                <c:pt idx="114">
-                  <c:v>37347</c:v>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v>37377</c:v>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v>37408</c:v>
-                </c:pt>
-                <c:pt idx="117">
-                  <c:v>37438</c:v>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v>37469</c:v>
-                </c:pt>
-                <c:pt idx="119">
-                  <c:v>37500</c:v>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v>37530</c:v>
-                </c:pt>
-                <c:pt idx="121">
-                  <c:v>37561</c:v>
-                </c:pt>
-                <c:pt idx="122">
-                  <c:v>37591</c:v>
-                </c:pt>
-                <c:pt idx="123">
-                  <c:v>37622</c:v>
-                </c:pt>
-                <c:pt idx="124">
-                  <c:v>37653</c:v>
-                </c:pt>
-                <c:pt idx="125">
-                  <c:v>37681</c:v>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v>37712</c:v>
-                </c:pt>
-                <c:pt idx="127">
-                  <c:v>37742</c:v>
-                </c:pt>
-                <c:pt idx="128">
-                  <c:v>37773</c:v>
-                </c:pt>
-                <c:pt idx="129">
-                  <c:v>37803</c:v>
-                </c:pt>
-                <c:pt idx="130">
-                  <c:v>37834</c:v>
-                </c:pt>
-                <c:pt idx="131">
-                  <c:v>37865</c:v>
-                </c:pt>
-                <c:pt idx="132">
-                  <c:v>37895</c:v>
-                </c:pt>
-                <c:pt idx="133">
-                  <c:v>37926</c:v>
-                </c:pt>
-                <c:pt idx="134">
-                  <c:v>37956</c:v>
-                </c:pt>
-                <c:pt idx="135">
-                  <c:v>37987</c:v>
-                </c:pt>
-                <c:pt idx="136">
-                  <c:v>38018</c:v>
-                </c:pt>
-                <c:pt idx="137">
-                  <c:v>38047</c:v>
-                </c:pt>
-                <c:pt idx="138">
-                  <c:v>38078</c:v>
-                </c:pt>
-                <c:pt idx="139">
-                  <c:v>38108</c:v>
-                </c:pt>
-                <c:pt idx="140">
-                  <c:v>38139</c:v>
-                </c:pt>
-                <c:pt idx="141">
-                  <c:v>38169</c:v>
-                </c:pt>
-                <c:pt idx="142">
-                  <c:v>38200</c:v>
-                </c:pt>
-                <c:pt idx="143">
-                  <c:v>38231</c:v>
-                </c:pt>
-                <c:pt idx="144">
-                  <c:v>38261</c:v>
-                </c:pt>
-                <c:pt idx="145">
-                  <c:v>38292</c:v>
-                </c:pt>
-                <c:pt idx="146">
-                  <c:v>38322</c:v>
-                </c:pt>
-                <c:pt idx="147">
-                  <c:v>38353</c:v>
-                </c:pt>
-                <c:pt idx="148">
-                  <c:v>38384</c:v>
-                </c:pt>
-                <c:pt idx="149">
-                  <c:v>38412</c:v>
-                </c:pt>
-                <c:pt idx="150">
-                  <c:v>38443</c:v>
-                </c:pt>
-                <c:pt idx="151">
-                  <c:v>38473</c:v>
-                </c:pt>
-                <c:pt idx="152">
-                  <c:v>38504</c:v>
-                </c:pt>
-                <c:pt idx="153">
-                  <c:v>38534</c:v>
-                </c:pt>
-                <c:pt idx="154">
-                  <c:v>38565</c:v>
-                </c:pt>
-                <c:pt idx="155">
-                  <c:v>38596</c:v>
-                </c:pt>
-                <c:pt idx="156">
-                  <c:v>38626</c:v>
-                </c:pt>
-                <c:pt idx="157">
-                  <c:v>38657</c:v>
-                </c:pt>
-                <c:pt idx="158">
-                  <c:v>38687</c:v>
-                </c:pt>
-                <c:pt idx="159">
-                  <c:v>38718</c:v>
-                </c:pt>
-                <c:pt idx="160">
-                  <c:v>38749</c:v>
-                </c:pt>
-                <c:pt idx="161">
-                  <c:v>38777</c:v>
-                </c:pt>
-                <c:pt idx="162">
-                  <c:v>38808</c:v>
-                </c:pt>
-                <c:pt idx="163">
-                  <c:v>38838</c:v>
-                </c:pt>
-                <c:pt idx="164">
-                  <c:v>38869</c:v>
-                </c:pt>
-                <c:pt idx="165">
-                  <c:v>38899</c:v>
-                </c:pt>
-                <c:pt idx="166">
-                  <c:v>38930</c:v>
-                </c:pt>
-                <c:pt idx="167">
-                  <c:v>38961</c:v>
-                </c:pt>
-                <c:pt idx="168">
-                  <c:v>38991</c:v>
-                </c:pt>
-                <c:pt idx="169">
-                  <c:v>39022</c:v>
-                </c:pt>
-                <c:pt idx="170">
-                  <c:v>39052</c:v>
-                </c:pt>
-                <c:pt idx="171">
-                  <c:v>39083</c:v>
-                </c:pt>
-                <c:pt idx="172">
-                  <c:v>39114</c:v>
-                </c:pt>
-                <c:pt idx="173">
-                  <c:v>39142</c:v>
-                </c:pt>
-                <c:pt idx="174">
-                  <c:v>39173</c:v>
-                </c:pt>
-                <c:pt idx="175">
-                  <c:v>39203</c:v>
-                </c:pt>
-                <c:pt idx="176">
-                  <c:v>39234</c:v>
-                </c:pt>
-                <c:pt idx="177">
-                  <c:v>39264</c:v>
-                </c:pt>
-                <c:pt idx="178">
-                  <c:v>39295</c:v>
-                </c:pt>
-                <c:pt idx="179">
-                  <c:v>39326</c:v>
-                </c:pt>
-                <c:pt idx="180">
-                  <c:v>39356</c:v>
-                </c:pt>
-                <c:pt idx="181">
-                  <c:v>39387</c:v>
-                </c:pt>
-                <c:pt idx="182">
-                  <c:v>39417</c:v>
-                </c:pt>
-                <c:pt idx="183">
-                  <c:v>39448</c:v>
-                </c:pt>
-                <c:pt idx="184">
-                  <c:v>39479</c:v>
-                </c:pt>
-                <c:pt idx="185">
-                  <c:v>39508</c:v>
-                </c:pt>
-                <c:pt idx="186">
-                  <c:v>39539</c:v>
-                </c:pt>
-                <c:pt idx="187">
-                  <c:v>39569</c:v>
-                </c:pt>
-                <c:pt idx="188">
-                  <c:v>39600</c:v>
-                </c:pt>
-                <c:pt idx="189">
-                  <c:v>39630</c:v>
-                </c:pt>
-                <c:pt idx="190">
-                  <c:v>39661</c:v>
-                </c:pt>
-                <c:pt idx="191">
-                  <c:v>39692</c:v>
-                </c:pt>
-                <c:pt idx="192">
-                  <c:v>39722</c:v>
-                </c:pt>
-                <c:pt idx="193">
-                  <c:v>39753</c:v>
-                </c:pt>
-                <c:pt idx="194">
-                  <c:v>39783</c:v>
-                </c:pt>
-                <c:pt idx="195">
-                  <c:v>39814</c:v>
-                </c:pt>
-                <c:pt idx="196">
-                  <c:v>39845</c:v>
-                </c:pt>
-                <c:pt idx="197">
-                  <c:v>39873</c:v>
-                </c:pt>
-                <c:pt idx="198">
-                  <c:v>39904</c:v>
-                </c:pt>
-                <c:pt idx="199">
-                  <c:v>39934</c:v>
-                </c:pt>
-                <c:pt idx="200">
-                  <c:v>39965</c:v>
-                </c:pt>
-                <c:pt idx="201">
-                  <c:v>39995</c:v>
-                </c:pt>
-                <c:pt idx="202">
-                  <c:v>40026</c:v>
-                </c:pt>
-                <c:pt idx="203">
-                  <c:v>40057</c:v>
-                </c:pt>
-                <c:pt idx="204">
-                  <c:v>40087</c:v>
-                </c:pt>
-                <c:pt idx="205">
-                  <c:v>40118</c:v>
-                </c:pt>
-                <c:pt idx="206">
-                  <c:v>40148</c:v>
-                </c:pt>
-                <c:pt idx="207">
-                  <c:v>40179</c:v>
-                </c:pt>
-                <c:pt idx="208">
-                  <c:v>40210</c:v>
-                </c:pt>
-                <c:pt idx="209">
-                  <c:v>40238</c:v>
-                </c:pt>
-                <c:pt idx="210">
-                  <c:v>40269</c:v>
-                </c:pt>
-                <c:pt idx="211">
-                  <c:v>40299</c:v>
-                </c:pt>
-                <c:pt idx="212">
-                  <c:v>40330</c:v>
-                </c:pt>
-                <c:pt idx="213">
-                  <c:v>40360</c:v>
-                </c:pt>
-                <c:pt idx="214">
-                  <c:v>40391</c:v>
-                </c:pt>
-                <c:pt idx="215">
-                  <c:v>40422</c:v>
-                </c:pt>
-                <c:pt idx="216">
-                  <c:v>40452</c:v>
-                </c:pt>
-                <c:pt idx="217">
-                  <c:v>40483</c:v>
-                </c:pt>
-                <c:pt idx="218">
-                  <c:v>40513</c:v>
-                </c:pt>
-                <c:pt idx="219">
-                  <c:v>40544</c:v>
-                </c:pt>
-                <c:pt idx="220">
-                  <c:v>40575</c:v>
-                </c:pt>
-                <c:pt idx="221">
-                  <c:v>40603</c:v>
-                </c:pt>
-                <c:pt idx="222">
-                  <c:v>40634</c:v>
-                </c:pt>
-                <c:pt idx="223">
-                  <c:v>40664</c:v>
-                </c:pt>
-                <c:pt idx="224">
-                  <c:v>40695</c:v>
-                </c:pt>
-                <c:pt idx="225">
-                  <c:v>40725</c:v>
-                </c:pt>
-                <c:pt idx="226">
-                  <c:v>40756</c:v>
-                </c:pt>
-                <c:pt idx="227">
-                  <c:v>40787</c:v>
-                </c:pt>
-                <c:pt idx="228">
-                  <c:v>40817</c:v>
-                </c:pt>
-                <c:pt idx="229">
-                  <c:v>40848</c:v>
-                </c:pt>
-                <c:pt idx="230">
-                  <c:v>40878</c:v>
-                </c:pt>
-                <c:pt idx="231">
-                  <c:v>40909</c:v>
-                </c:pt>
-                <c:pt idx="232">
-                  <c:v>40940</c:v>
-                </c:pt>
-                <c:pt idx="233">
-                  <c:v>40969</c:v>
-                </c:pt>
-                <c:pt idx="234">
-                  <c:v>41000</c:v>
-                </c:pt>
-                <c:pt idx="235">
-                  <c:v>41030</c:v>
-                </c:pt>
-                <c:pt idx="236">
-                  <c:v>41061</c:v>
-                </c:pt>
-                <c:pt idx="237">
-                  <c:v>41091</c:v>
-                </c:pt>
-                <c:pt idx="238">
-                  <c:v>41122</c:v>
-                </c:pt>
-                <c:pt idx="239">
-                  <c:v>41153</c:v>
-                </c:pt>
-                <c:pt idx="240">
-                  <c:v>41183</c:v>
-                </c:pt>
-                <c:pt idx="241">
-                  <c:v>41214</c:v>
-                </c:pt>
-                <c:pt idx="242">
-                  <c:v>41244</c:v>
-                </c:pt>
-                <c:pt idx="243">
-                  <c:v>41275</c:v>
-                </c:pt>
-                <c:pt idx="244">
-                  <c:v>41306</c:v>
-                </c:pt>
-                <c:pt idx="245">
-                  <c:v>41334</c:v>
-                </c:pt>
-                <c:pt idx="246">
-                  <c:v>41365</c:v>
-                </c:pt>
-                <c:pt idx="247">
-                  <c:v>41395</c:v>
-                </c:pt>
-                <c:pt idx="248">
-                  <c:v>41426</c:v>
-                </c:pt>
-                <c:pt idx="249">
-                  <c:v>41456</c:v>
-                </c:pt>
-                <c:pt idx="250">
-                  <c:v>41487</c:v>
-                </c:pt>
-                <c:pt idx="251">
-                  <c:v>41518</c:v>
-                </c:pt>
-                <c:pt idx="252">
-                  <c:v>41548</c:v>
-                </c:pt>
-                <c:pt idx="253">
-                  <c:v>41579</c:v>
-                </c:pt>
-                <c:pt idx="254">
-                  <c:v>41609</c:v>
-                </c:pt>
-                <c:pt idx="255">
-                  <c:v>41640</c:v>
-                </c:pt>
-                <c:pt idx="256">
-                  <c:v>41671</c:v>
-                </c:pt>
-                <c:pt idx="257">
-                  <c:v>41699</c:v>
-                </c:pt>
-                <c:pt idx="258">
-                  <c:v>41730</c:v>
-                </c:pt>
-                <c:pt idx="259">
-                  <c:v>41760</c:v>
-                </c:pt>
-                <c:pt idx="260">
-                  <c:v>41791</c:v>
-                </c:pt>
-                <c:pt idx="261">
-                  <c:v>41821</c:v>
-                </c:pt>
-                <c:pt idx="262">
-                  <c:v>41852</c:v>
-                </c:pt>
-                <c:pt idx="263">
-                  <c:v>41883</c:v>
-                </c:pt>
-                <c:pt idx="264">
-                  <c:v>41913</c:v>
-                </c:pt>
-                <c:pt idx="265">
-                  <c:v>41944</c:v>
-                </c:pt>
-                <c:pt idx="266">
-                  <c:v>41974</c:v>
-                </c:pt>
-                <c:pt idx="267">
-                  <c:v>42005</c:v>
-                </c:pt>
-                <c:pt idx="268">
-                  <c:v>42036</c:v>
-                </c:pt>
-                <c:pt idx="269">
-                  <c:v>42064</c:v>
-                </c:pt>
-                <c:pt idx="270">
-                  <c:v>42095</c:v>
-                </c:pt>
-                <c:pt idx="271">
-                  <c:v>42125</c:v>
-                </c:pt>
-                <c:pt idx="272">
-                  <c:v>42156</c:v>
-                </c:pt>
-                <c:pt idx="273">
-                  <c:v>42186</c:v>
-                </c:pt>
-                <c:pt idx="274">
-                  <c:v>42217</c:v>
-                </c:pt>
-                <c:pt idx="275">
-                  <c:v>42248</c:v>
-                </c:pt>
-                <c:pt idx="276">
-                  <c:v>42278</c:v>
-                </c:pt>
-                <c:pt idx="277">
-                  <c:v>42309</c:v>
-                </c:pt>
-                <c:pt idx="278">
-                  <c:v>42339</c:v>
-                </c:pt>
-                <c:pt idx="279">
-                  <c:v>42370</c:v>
-                </c:pt>
-                <c:pt idx="280">
-                  <c:v>42401</c:v>
-                </c:pt>
-                <c:pt idx="281">
-                  <c:v>42430</c:v>
-                </c:pt>
-                <c:pt idx="282">
-                  <c:v>42461</c:v>
-                </c:pt>
-                <c:pt idx="283">
-                  <c:v>42491</c:v>
-                </c:pt>
-                <c:pt idx="284">
-                  <c:v>42522</c:v>
-                </c:pt>
-                <c:pt idx="285">
-                  <c:v>42552</c:v>
-                </c:pt>
-                <c:pt idx="286">
-                  <c:v>42583</c:v>
-                </c:pt>
-                <c:pt idx="287">
-                  <c:v>42614</c:v>
-                </c:pt>
-                <c:pt idx="288">
-                  <c:v>42644</c:v>
-                </c:pt>
-                <c:pt idx="289">
-                  <c:v>42675</c:v>
-                </c:pt>
-                <c:pt idx="290">
-                  <c:v>42705</c:v>
-                </c:pt>
-                <c:pt idx="291">
-                  <c:v>42736</c:v>
-                </c:pt>
-                <c:pt idx="292">
-                  <c:v>42767</c:v>
-                </c:pt>
-                <c:pt idx="293">
-                  <c:v>42795</c:v>
-                </c:pt>
-                <c:pt idx="294">
-                  <c:v>42826</c:v>
-                </c:pt>
-                <c:pt idx="295">
-                  <c:v>42856</c:v>
-                </c:pt>
-                <c:pt idx="296">
-                  <c:v>42887</c:v>
-                </c:pt>
-                <c:pt idx="297">
-                  <c:v>42917</c:v>
-                </c:pt>
-                <c:pt idx="298">
-                  <c:v>42948</c:v>
-                </c:pt>
-                <c:pt idx="299">
-                  <c:v>42979</c:v>
-                </c:pt>
-                <c:pt idx="300">
-                  <c:v>43009</c:v>
-                </c:pt>
-                <c:pt idx="301">
-                  <c:v>43040</c:v>
-                </c:pt>
-                <c:pt idx="302">
-                  <c:v>43070</c:v>
-                </c:pt>
-                <c:pt idx="303">
-                  <c:v>43101</c:v>
-                </c:pt>
-                <c:pt idx="304">
-                  <c:v>43132</c:v>
-                </c:pt>
-                <c:pt idx="305">
-                  <c:v>43160</c:v>
-                </c:pt>
-                <c:pt idx="306">
-                  <c:v>43191</c:v>
-                </c:pt>
-                <c:pt idx="307">
-                  <c:v>43221</c:v>
-                </c:pt>
-                <c:pt idx="308">
-                  <c:v>43252</c:v>
-                </c:pt>
-                <c:pt idx="309">
-                  <c:v>43282</c:v>
-                </c:pt>
-                <c:pt idx="310">
-                  <c:v>43313</c:v>
-                </c:pt>
-                <c:pt idx="311">
-                  <c:v>43344</c:v>
-                </c:pt>
-                <c:pt idx="312">
-                  <c:v>43374</c:v>
-                </c:pt>
-                <c:pt idx="313">
-                  <c:v>43405</c:v>
-                </c:pt>
-                <c:pt idx="314">
-                  <c:v>43435</c:v>
-                </c:pt>
-                <c:pt idx="315">
-                  <c:v>43466</c:v>
-                </c:pt>
-                <c:pt idx="316">
-                  <c:v>43497</c:v>
-                </c:pt>
-                <c:pt idx="317">
-                  <c:v>43525</c:v>
-                </c:pt>
-                <c:pt idx="318">
-                  <c:v>43556</c:v>
-                </c:pt>
-                <c:pt idx="319">
-                  <c:v>43586</c:v>
-                </c:pt>
-                <c:pt idx="320">
-                  <c:v>43617</c:v>
-                </c:pt>
-                <c:pt idx="321">
-                  <c:v>43647</c:v>
-                </c:pt>
-                <c:pt idx="322">
-                  <c:v>43678</c:v>
-                </c:pt>
-                <c:pt idx="323">
-                  <c:v>43709</c:v>
-                </c:pt>
-                <c:pt idx="324">
-                  <c:v>43739</c:v>
-                </c:pt>
-                <c:pt idx="325">
-                  <c:v>43770</c:v>
-                </c:pt>
-                <c:pt idx="326">
-                  <c:v>43800</c:v>
-                </c:pt>
-                <c:pt idx="327">
-                  <c:v>43831</c:v>
-                </c:pt>
-                <c:pt idx="328">
-                  <c:v>43862</c:v>
-                </c:pt>
-                <c:pt idx="329">
-                  <c:v>43891</c:v>
-                </c:pt>
-                <c:pt idx="330">
-                  <c:v>43922</c:v>
-                </c:pt>
-                <c:pt idx="331">
-                  <c:v>43952</c:v>
-                </c:pt>
-                <c:pt idx="332">
-                  <c:v>43983</c:v>
-                </c:pt>
-                <c:pt idx="333">
-                  <c:v>44013</c:v>
-                </c:pt>
-                <c:pt idx="334">
-                  <c:v>44044</c:v>
-                </c:pt>
-                <c:pt idx="335">
-                  <c:v>44075</c:v>
-                </c:pt>
-                <c:pt idx="336">
-                  <c:v>44105</c:v>
-                </c:pt>
-                <c:pt idx="337">
-                  <c:v>44136</c:v>
-                </c:pt>
-                <c:pt idx="338">
-                  <c:v>44166</c:v>
-                </c:pt>
-                <c:pt idx="339">
-                  <c:v>44197</c:v>
-                </c:pt>
-                <c:pt idx="340">
-                  <c:v>44228</c:v>
-                </c:pt>
-                <c:pt idx="341">
-                  <c:v>44256</c:v>
-                </c:pt>
-                <c:pt idx="342">
-                  <c:v>44287</c:v>
-                </c:pt>
-                <c:pt idx="343">
-                  <c:v>44317</c:v>
-                </c:pt>
-                <c:pt idx="344">
-                  <c:v>44348</c:v>
-                </c:pt>
-                <c:pt idx="345">
-                  <c:v>44378</c:v>
-                </c:pt>
-                <c:pt idx="346">
-                  <c:v>44409</c:v>
-                </c:pt>
-                <c:pt idx="347">
-                  <c:v>44440</c:v>
-                </c:pt>
-                <c:pt idx="348">
-                  <c:v>44470</c:v>
-                </c:pt>
-                <c:pt idx="349">
-                  <c:v>44501</c:v>
-                </c:pt>
-                <c:pt idx="350">
-                  <c:v>44531</c:v>
-                </c:pt>
-                <c:pt idx="351">
-                  <c:v>44562</c:v>
-                </c:pt>
-                <c:pt idx="352">
-                  <c:v>44593</c:v>
-                </c:pt>
-                <c:pt idx="353">
-                  <c:v>44621</c:v>
-                </c:pt>
-                <c:pt idx="354">
-                  <c:v>44652</c:v>
-                </c:pt>
-                <c:pt idx="355">
-                  <c:v>44682</c:v>
-                </c:pt>
-                <c:pt idx="356">
-                  <c:v>44713</c:v>
-                </c:pt>
-                <c:pt idx="357">
-                  <c:v>44743</c:v>
-                </c:pt>
-                <c:pt idx="358">
-                  <c:v>44774</c:v>
-                </c:pt>
-                <c:pt idx="359">
-                  <c:v>44805</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'اوره بلندمدت'!$B$2:$B$361</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="360"/>
-                <c:pt idx="0">
-                  <c:v>116.88</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>107.5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>103.75</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>102.5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>102.5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>86.2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>81</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>81</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>81</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>81</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>81</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>81</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>81</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>82.8</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>85.5</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>85.5</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>85.5</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>98.63</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>103.5</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>103.5</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>103.5</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>106.5</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>88</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>88</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>88</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>88</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>88</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>159.6</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>177.5</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>191.25</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>205</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>159</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>160.4</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>169.5</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>172.13</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>184.5</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>187</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>181.4</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>172.25</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>172.63</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>174.5</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>173.5</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>160.38</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>148</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>135</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>113.13</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>108.5</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>112.5</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>102.5</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>88.3</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>87.5</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>90.63</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>86.25</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>77.5</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>84.5</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>95</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>88.4</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>86</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>85.5</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>83.63</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>75.63</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>70.7</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>65.5</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>64.5</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>75.5</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>64.5</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>64.900000000000006</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>63.75</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>62.75</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>65.7</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>67.5</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>65.38</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>66</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>66.83</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>77.400000000000006</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>90.13</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>88.75</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>83.25</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>91</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>105.13</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>121.7</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>133.38</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>113.88</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>111.1</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>99.38</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>96</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>121</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>105.25</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>98.88</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>95.3</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>85</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>87.5</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>87.5</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>88.75</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>94.5</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>96.1</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>96.5</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>101.17</c:v>
-                </c:pt>
-                <c:pt idx="111">
-                  <c:v>104.13</c:v>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v>99.63</c:v>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v>90.25</c:v>
-                </c:pt>
-                <c:pt idx="114">
-                  <c:v>84.7</c:v>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v>85.5</c:v>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v>92.75</c:v>
-                </c:pt>
-                <c:pt idx="117">
-                  <c:v>94.2</c:v>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v>105</c:v>
-                </c:pt>
-                <c:pt idx="119">
-                  <c:v>93</c:v>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v>92.25</c:v>
-                </c:pt>
-                <c:pt idx="121">
-                  <c:v>92.25</c:v>
-                </c:pt>
-                <c:pt idx="122">
-                  <c:v>99.38</c:v>
-                </c:pt>
-                <c:pt idx="123">
-                  <c:v>112</c:v>
-                </c:pt>
-                <c:pt idx="124">
-                  <c:v>132.13</c:v>
-                </c:pt>
-                <c:pt idx="125">
-                  <c:v>138.9</c:v>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v>118.63</c:v>
-                </c:pt>
-                <c:pt idx="127">
-                  <c:v>128.13</c:v>
-                </c:pt>
-                <c:pt idx="128">
-                  <c:v>133.9</c:v>
-                </c:pt>
-                <c:pt idx="129">
-                  <c:v>142.75</c:v>
-                </c:pt>
-                <c:pt idx="130">
-                  <c:v>141.5</c:v>
-                </c:pt>
-                <c:pt idx="131">
-                  <c:v>146.80000000000001</c:v>
-                </c:pt>
-                <c:pt idx="132">
-                  <c:v>150.63</c:v>
-                </c:pt>
-                <c:pt idx="133">
-                  <c:v>153.5</c:v>
-                </c:pt>
-                <c:pt idx="134">
-                  <c:v>159.38</c:v>
-                </c:pt>
-                <c:pt idx="135">
-                  <c:v>160.25</c:v>
-                </c:pt>
-                <c:pt idx="136">
-                  <c:v>134.5</c:v>
-                </c:pt>
-                <c:pt idx="137">
-                  <c:v>130.5</c:v>
-                </c:pt>
-                <c:pt idx="138">
-                  <c:v>128.38</c:v>
-                </c:pt>
-                <c:pt idx="139">
-                  <c:v>135.9</c:v>
-                </c:pt>
-                <c:pt idx="140">
-                  <c:v>158.25</c:v>
-                </c:pt>
-                <c:pt idx="141">
-                  <c:v>185</c:v>
-                </c:pt>
-                <c:pt idx="142">
-                  <c:v>196.2</c:v>
-                </c:pt>
-                <c:pt idx="143">
-                  <c:v>218.13</c:v>
-                </c:pt>
-                <c:pt idx="144">
-                  <c:v>242.13</c:v>
-                </c:pt>
-                <c:pt idx="145">
-                  <c:v>224.5</c:v>
-                </c:pt>
-                <c:pt idx="146">
-                  <c:v>185.25</c:v>
-                </c:pt>
-                <c:pt idx="147">
-                  <c:v>184.6</c:v>
-                </c:pt>
-                <c:pt idx="148">
-                  <c:v>185.75</c:v>
-                </c:pt>
-                <c:pt idx="149">
-                  <c:v>217.13</c:v>
-                </c:pt>
-                <c:pt idx="150">
-                  <c:v>242.13</c:v>
-                </c:pt>
-                <c:pt idx="151">
-                  <c:v>256</c:v>
-                </c:pt>
-                <c:pt idx="152">
-                  <c:v>217.5</c:v>
-                </c:pt>
-                <c:pt idx="153">
-                  <c:v>221.88</c:v>
-                </c:pt>
-                <c:pt idx="154">
-                  <c:v>208.5</c:v>
-                </c:pt>
-                <c:pt idx="155">
-                  <c:v>210.38</c:v>
-                </c:pt>
-                <c:pt idx="156">
-                  <c:v>215.5</c:v>
-                </c:pt>
-                <c:pt idx="157">
-                  <c:v>235</c:v>
-                </c:pt>
-                <c:pt idx="158">
-                  <c:v>213.88</c:v>
-                </c:pt>
-                <c:pt idx="159">
-                  <c:v>202.3</c:v>
-                </c:pt>
-                <c:pt idx="160">
-                  <c:v>213.88</c:v>
-                </c:pt>
-                <c:pt idx="161">
-                  <c:v>243.13</c:v>
-                </c:pt>
-                <c:pt idx="162">
-                  <c:v>247.5</c:v>
-                </c:pt>
-                <c:pt idx="163">
-                  <c:v>229.5</c:v>
-                </c:pt>
-                <c:pt idx="164">
-                  <c:v>210</c:v>
-                </c:pt>
-                <c:pt idx="165">
-                  <c:v>205.5</c:v>
-                </c:pt>
-                <c:pt idx="166">
-                  <c:v>210.5</c:v>
-                </c:pt>
-                <c:pt idx="167">
-                  <c:v>215.13</c:v>
-                </c:pt>
-                <c:pt idx="168">
-                  <c:v>209.2</c:v>
-                </c:pt>
-                <c:pt idx="169">
-                  <c:v>227.38</c:v>
-                </c:pt>
-                <c:pt idx="170">
-                  <c:v>251.67</c:v>
-                </c:pt>
-                <c:pt idx="171">
-                  <c:v>265</c:v>
-                </c:pt>
-                <c:pt idx="172">
-                  <c:v>299.38</c:v>
-                </c:pt>
-                <c:pt idx="173">
-                  <c:v>318.13</c:v>
-                </c:pt>
-                <c:pt idx="174">
-                  <c:v>291</c:v>
-                </c:pt>
-                <c:pt idx="175">
-                  <c:v>293.13</c:v>
-                </c:pt>
-                <c:pt idx="176">
-                  <c:v>291.88</c:v>
-                </c:pt>
-                <c:pt idx="177">
-                  <c:v>269.5</c:v>
-                </c:pt>
-                <c:pt idx="178">
-                  <c:v>260.63</c:v>
-                </c:pt>
-                <c:pt idx="179">
-                  <c:v>305</c:v>
-                </c:pt>
-                <c:pt idx="180">
-                  <c:v>323.75</c:v>
-                </c:pt>
-                <c:pt idx="181">
-                  <c:v>366.25</c:v>
-                </c:pt>
-                <c:pt idx="182">
-                  <c:v>401.67</c:v>
-                </c:pt>
-                <c:pt idx="183">
-                  <c:v>376.63</c:v>
-                </c:pt>
-                <c:pt idx="184">
-                  <c:v>328.13</c:v>
-                </c:pt>
-                <c:pt idx="185">
-                  <c:v>371</c:v>
-                </c:pt>
-                <c:pt idx="186">
-                  <c:v>462.5</c:v>
-                </c:pt>
-                <c:pt idx="187">
-                  <c:v>633.75</c:v>
-                </c:pt>
-                <c:pt idx="188">
-                  <c:v>642</c:v>
-                </c:pt>
-                <c:pt idx="189">
-                  <c:v>733.75</c:v>
-                </c:pt>
-                <c:pt idx="190">
-                  <c:v>785</c:v>
-                </c:pt>
-                <c:pt idx="191">
-                  <c:v>744.5</c:v>
-                </c:pt>
-                <c:pt idx="192">
-                  <c:v>575</c:v>
-                </c:pt>
-                <c:pt idx="193">
-                  <c:v>287.5</c:v>
-                </c:pt>
-                <c:pt idx="194">
-                  <c:v>240</c:v>
-                </c:pt>
-                <c:pt idx="195">
-                  <c:v>273.75</c:v>
-                </c:pt>
-                <c:pt idx="196">
-                  <c:v>281.25</c:v>
-                </c:pt>
-                <c:pt idx="197">
-                  <c:v>268.5</c:v>
-                </c:pt>
-                <c:pt idx="198">
-                  <c:v>245.63</c:v>
-                </c:pt>
-                <c:pt idx="199">
-                  <c:v>236.25</c:v>
-                </c:pt>
-                <c:pt idx="200">
-                  <c:v>239.7</c:v>
-                </c:pt>
-                <c:pt idx="201">
-                  <c:v>243.75</c:v>
-                </c:pt>
-                <c:pt idx="202">
-                  <c:v>251.5</c:v>
-                </c:pt>
-                <c:pt idx="203">
-                  <c:v>232.25</c:v>
-                </c:pt>
-                <c:pt idx="204">
-                  <c:v>234.88</c:v>
-                </c:pt>
-                <c:pt idx="205">
-                  <c:v>243.5</c:v>
-                </c:pt>
-                <c:pt idx="206">
-                  <c:v>262</c:v>
-                </c:pt>
-                <c:pt idx="207">
-                  <c:v>266.5</c:v>
-                </c:pt>
-                <c:pt idx="208">
-                  <c:v>297.5</c:v>
-                </c:pt>
-                <c:pt idx="209">
-                  <c:v>278.7</c:v>
-                </c:pt>
-                <c:pt idx="210">
-                  <c:v>253.75</c:v>
-                </c:pt>
-                <c:pt idx="211">
-                  <c:v>234</c:v>
-                </c:pt>
-                <c:pt idx="212">
-                  <c:v>226.25</c:v>
-                </c:pt>
-                <c:pt idx="213">
-                  <c:v>259.38</c:v>
-                </c:pt>
-                <c:pt idx="214">
-                  <c:v>263.5</c:v>
-                </c:pt>
-                <c:pt idx="215">
-                  <c:v>308.75</c:v>
-                </c:pt>
-                <c:pt idx="216">
-                  <c:v>332.5</c:v>
-                </c:pt>
-                <c:pt idx="217">
-                  <c:v>365.4</c:v>
-                </c:pt>
-                <c:pt idx="218">
-                  <c:v>380.63</c:v>
-                </c:pt>
-                <c:pt idx="219">
-                  <c:v>378.5</c:v>
-                </c:pt>
-                <c:pt idx="220">
-                  <c:v>297.5</c:v>
-                </c:pt>
-                <c:pt idx="221">
-                  <c:v>278.7</c:v>
-                </c:pt>
-                <c:pt idx="222">
-                  <c:v>253.75</c:v>
-                </c:pt>
-                <c:pt idx="223">
-                  <c:v>234</c:v>
-                </c:pt>
-                <c:pt idx="224">
-                  <c:v>478.75</c:v>
-                </c:pt>
-                <c:pt idx="225">
-                  <c:v>483.75</c:v>
-                </c:pt>
-                <c:pt idx="226">
-                  <c:v>475.5</c:v>
-                </c:pt>
-                <c:pt idx="227">
-                  <c:v>508.75</c:v>
-                </c:pt>
-                <c:pt idx="228">
-                  <c:v>493.5</c:v>
-                </c:pt>
-                <c:pt idx="229">
-                  <c:v>481.25</c:v>
-                </c:pt>
-                <c:pt idx="230">
-                  <c:v>423.13</c:v>
-                </c:pt>
-                <c:pt idx="231">
-                  <c:v>368</c:v>
-                </c:pt>
-                <c:pt idx="232">
-                  <c:v>375</c:v>
-                </c:pt>
-                <c:pt idx="233">
-                  <c:v>393.13</c:v>
-                </c:pt>
-                <c:pt idx="234">
-                  <c:v>494.38</c:v>
-                </c:pt>
-                <c:pt idx="235">
-                  <c:v>513.13</c:v>
-                </c:pt>
-                <c:pt idx="236">
-                  <c:v>456.88</c:v>
-                </c:pt>
-                <c:pt idx="237">
-                  <c:v>307.5</c:v>
-                </c:pt>
-                <c:pt idx="238">
-                  <c:v>382.5</c:v>
-                </c:pt>
-                <c:pt idx="239">
-                  <c:v>384.38</c:v>
-                </c:pt>
-                <c:pt idx="240">
-                  <c:v>349</c:v>
-                </c:pt>
-                <c:pt idx="241">
-                  <c:v>383.5</c:v>
-                </c:pt>
-                <c:pt idx="242">
-                  <c:v>375.83</c:v>
-                </c:pt>
-                <c:pt idx="243">
-                  <c:v>380</c:v>
-                </c:pt>
-                <c:pt idx="244">
-                  <c:v>415.63</c:v>
-                </c:pt>
-                <c:pt idx="245">
-                  <c:v>395.63</c:v>
-                </c:pt>
-                <c:pt idx="246">
-                  <c:v>365.63</c:v>
-                </c:pt>
-                <c:pt idx="247">
-                  <c:v>358.13</c:v>
-                </c:pt>
-                <c:pt idx="248">
-                  <c:v>329.38</c:v>
-                </c:pt>
-                <c:pt idx="249">
-                  <c:v>312.5</c:v>
-                </c:pt>
-                <c:pt idx="250">
-                  <c:v>310.63</c:v>
-                </c:pt>
-                <c:pt idx="251">
-                  <c:v>301</c:v>
-                </c:pt>
-                <c:pt idx="252">
-                  <c:v>296.88</c:v>
-                </c:pt>
-                <c:pt idx="253">
-                  <c:v>305</c:v>
-                </c:pt>
-                <c:pt idx="254">
-                  <c:v>305</c:v>
-                </c:pt>
-                <c:pt idx="255">
-                  <c:v>330</c:v>
-                </c:pt>
-                <c:pt idx="256">
-                  <c:v>353.13</c:v>
-                </c:pt>
-                <c:pt idx="257">
-                  <c:v>327.5</c:v>
-                </c:pt>
-                <c:pt idx="258">
-                  <c:v>260</c:v>
-                </c:pt>
-                <c:pt idx="259">
-                  <c:v>265</c:v>
-                </c:pt>
-                <c:pt idx="260">
-                  <c:v>288.75</c:v>
-                </c:pt>
-                <c:pt idx="261">
-                  <c:v>305</c:v>
-                </c:pt>
-                <c:pt idx="262">
-                  <c:v>311.25</c:v>
-                </c:pt>
-                <c:pt idx="263">
-                  <c:v>317.5</c:v>
-                </c:pt>
-                <c:pt idx="264">
-                  <c:v>317.5</c:v>
-                </c:pt>
-                <c:pt idx="265">
-                  <c:v>317.5</c:v>
-                </c:pt>
-                <c:pt idx="266">
-                  <c:v>308.13</c:v>
-                </c:pt>
-                <c:pt idx="267">
-                  <c:v>305</c:v>
-                </c:pt>
-                <c:pt idx="268">
-                  <c:v>305</c:v>
-                </c:pt>
-                <c:pt idx="269">
-                  <c:v>295.5</c:v>
-                </c:pt>
-                <c:pt idx="270">
-                  <c:v>260</c:v>
-                </c:pt>
-                <c:pt idx="271">
-                  <c:v>265</c:v>
-                </c:pt>
-                <c:pt idx="272">
-                  <c:v>288.75</c:v>
-                </c:pt>
-                <c:pt idx="273">
-                  <c:v>283.75</c:v>
-                </c:pt>
-                <c:pt idx="274">
-                  <c:v>274.63</c:v>
-                </c:pt>
-                <c:pt idx="275">
-                  <c:v>279.38</c:v>
-                </c:pt>
-                <c:pt idx="276">
-                  <c:v>250.63</c:v>
-                </c:pt>
-                <c:pt idx="277">
-                  <c:v>263.63</c:v>
-                </c:pt>
-                <c:pt idx="278">
-                  <c:v>264</c:v>
-                </c:pt>
-                <c:pt idx="279">
-                  <c:v>233.88</c:v>
-                </c:pt>
-                <c:pt idx="280">
-                  <c:v>191.88</c:v>
-                </c:pt>
-                <c:pt idx="281">
-                  <c:v>201.75</c:v>
-                </c:pt>
-                <c:pt idx="282">
-                  <c:v>196.25</c:v>
-                </c:pt>
-                <c:pt idx="283">
-                  <c:v>198.38</c:v>
-                </c:pt>
-                <c:pt idx="284">
-                  <c:v>142.63</c:v>
-                </c:pt>
-                <c:pt idx="285">
-                  <c:v>181</c:v>
-                </c:pt>
-                <c:pt idx="286">
-                  <c:v>186.25</c:v>
-                </c:pt>
-                <c:pt idx="287">
-                  <c:v>187.3</c:v>
-                </c:pt>
-                <c:pt idx="288">
-                  <c:v>187.5</c:v>
-                </c:pt>
-                <c:pt idx="289">
-                  <c:v>205</c:v>
-                </c:pt>
-                <c:pt idx="290">
-                  <c:v>217.75</c:v>
-                </c:pt>
-                <c:pt idx="291">
-                  <c:v>233.75</c:v>
-                </c:pt>
-                <c:pt idx="292">
-                  <c:v>191.88</c:v>
-                </c:pt>
-                <c:pt idx="293">
-                  <c:v>223.5</c:v>
-                </c:pt>
-                <c:pt idx="294">
-                  <c:v>207.88</c:v>
-                </c:pt>
-                <c:pt idx="295">
-                  <c:v>178.75</c:v>
-                </c:pt>
-                <c:pt idx="296">
-                  <c:v>191</c:v>
-                </c:pt>
-                <c:pt idx="297">
-                  <c:v>181</c:v>
-                </c:pt>
-                <c:pt idx="298">
-                  <c:v>192.63</c:v>
-                </c:pt>
-                <c:pt idx="299">
-                  <c:v>219</c:v>
-                </c:pt>
-                <c:pt idx="300">
-                  <c:v>252.5</c:v>
-                </c:pt>
-                <c:pt idx="301">
-                  <c:v>280</c:v>
-                </c:pt>
-                <c:pt idx="302">
-                  <c:v>214.63</c:v>
-                </c:pt>
-                <c:pt idx="303">
-                  <c:v>219.63</c:v>
-                </c:pt>
-                <c:pt idx="304">
-                  <c:v>232.5</c:v>
-                </c:pt>
-                <c:pt idx="305">
-                  <c:v>232.5</c:v>
-                </c:pt>
-                <c:pt idx="306">
-                  <c:v>230.63</c:v>
-                </c:pt>
-                <c:pt idx="307">
-                  <c:v>221.88</c:v>
-                </c:pt>
-                <c:pt idx="308">
-                  <c:v>224</c:v>
-                </c:pt>
-                <c:pt idx="309">
-                  <c:v>252.5</c:v>
-                </c:pt>
-                <c:pt idx="310">
-                  <c:v>260</c:v>
-                </c:pt>
-                <c:pt idx="311">
-                  <c:v>267.5</c:v>
-                </c:pt>
-                <c:pt idx="312">
-                  <c:v>270</c:v>
-                </c:pt>
-                <c:pt idx="313">
-                  <c:v>305.60000000000002</c:v>
-                </c:pt>
-                <c:pt idx="314">
-                  <c:v>276.67</c:v>
-                </c:pt>
-                <c:pt idx="315">
-                  <c:v>260</c:v>
-                </c:pt>
-                <c:pt idx="316">
-                  <c:v>250.63</c:v>
-                </c:pt>
-                <c:pt idx="317">
-                  <c:v>247.5</c:v>
-                </c:pt>
-                <c:pt idx="318">
-                  <c:v>247.5</c:v>
-                </c:pt>
-                <c:pt idx="319">
-                  <c:v>247.5</c:v>
-                </c:pt>
-                <c:pt idx="320">
-                  <c:v>247.5</c:v>
-                </c:pt>
-                <c:pt idx="321">
-                  <c:v>263.5</c:v>
-                </c:pt>
-                <c:pt idx="322">
-                  <c:v>262.5</c:v>
-                </c:pt>
-                <c:pt idx="323">
-                  <c:v>237.75</c:v>
-                </c:pt>
-                <c:pt idx="324">
-                  <c:v>237</c:v>
-                </c:pt>
-                <c:pt idx="325">
-                  <c:v>224.5</c:v>
-                </c:pt>
-                <c:pt idx="326">
-                  <c:v>217.5</c:v>
-                </c:pt>
-                <c:pt idx="327">
-                  <c:v>215.4</c:v>
-                </c:pt>
-                <c:pt idx="328">
-                  <c:v>214.38</c:v>
-                </c:pt>
-                <c:pt idx="329">
-                  <c:v>231.13</c:v>
-                </c:pt>
-                <c:pt idx="330">
-                  <c:v>235</c:v>
-                </c:pt>
-                <c:pt idx="331">
-                  <c:v>201.9</c:v>
-                </c:pt>
-                <c:pt idx="332">
-                  <c:v>202</c:v>
-                </c:pt>
-                <c:pt idx="333">
-                  <c:v>214.4</c:v>
-                </c:pt>
-                <c:pt idx="334">
-                  <c:v>249.5</c:v>
-                </c:pt>
-                <c:pt idx="335">
-                  <c:v>250.5</c:v>
-                </c:pt>
-                <c:pt idx="336">
-                  <c:v>245</c:v>
-                </c:pt>
-                <c:pt idx="337">
-                  <c:v>245</c:v>
-                </c:pt>
-                <c:pt idx="338">
-                  <c:v>245</c:v>
-                </c:pt>
-                <c:pt idx="339">
-                  <c:v>265</c:v>
-                </c:pt>
-                <c:pt idx="340">
-                  <c:v>335</c:v>
-                </c:pt>
-                <c:pt idx="341">
-                  <c:v>352.88</c:v>
-                </c:pt>
-                <c:pt idx="342">
-                  <c:v>328.1</c:v>
-                </c:pt>
-                <c:pt idx="343">
-                  <c:v>331.63</c:v>
-                </c:pt>
-                <c:pt idx="344">
-                  <c:v>393.25</c:v>
-                </c:pt>
-                <c:pt idx="345">
-                  <c:v>441.5</c:v>
-                </c:pt>
-                <c:pt idx="346">
-                  <c:v>446.88</c:v>
-                </c:pt>
-                <c:pt idx="347">
-                  <c:v>418.75</c:v>
-                </c:pt>
-                <c:pt idx="348">
-                  <c:v>695</c:v>
-                </c:pt>
-                <c:pt idx="349">
-                  <c:v>900.5</c:v>
-                </c:pt>
-                <c:pt idx="350">
-                  <c:v>890</c:v>
-                </c:pt>
-                <c:pt idx="351">
-                  <c:v>846.38</c:v>
-                </c:pt>
-                <c:pt idx="352">
-                  <c:v>744.17</c:v>
-                </c:pt>
-                <c:pt idx="353">
-                  <c:v>872.5</c:v>
-                </c:pt>
-                <c:pt idx="354">
-                  <c:v>925</c:v>
-                </c:pt>
-                <c:pt idx="355">
-                  <c:v>707.5</c:v>
-                </c:pt>
-                <c:pt idx="356">
-                  <c:v>690</c:v>
-                </c:pt>
-                <c:pt idx="357">
-                  <c:v>601</c:v>
-                </c:pt>
-                <c:pt idx="358">
-                  <c:v>591.25</c:v>
-                </c:pt>
-                <c:pt idx="359">
-                  <c:v>678</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-3883-4AE3-B3C2-099301B5B0EA}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="947277904"/>
-        <c:axId val="947272496"/>
-      </c:lineChart>
-      <c:dateAx>
-        <c:axId val="947277904"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:lumMod val="95000"/>
-                <a:alpha val="10000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="85000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="947272496"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblOffset val="100"/>
-        <c:baseTimeUnit val="months"/>
-      </c:dateAx>
-      <c:valAx>
-        <c:axId val="947272496"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
-                  <a:alpha val="10000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="85000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="947277904"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:gradFill flip="none" rotWithShape="1">
-      <a:gsLst>
-        <a:gs pos="0">
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:gs>
-        <a:gs pos="100000">
-          <a:schemeClr val="dk1">
-            <a:lumMod val="85000"/>
-            <a:lumOff val="15000"/>
-          </a:schemeClr>
-        </a:gs>
-      </a:gsLst>
-      <a:path path="circle">
-        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-      </a:path>
-      <a:tileRect/>
-    </a:gradFill>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="10000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:gradFill flip="none" rotWithShape="1">
-        <a:gsLst>
-          <a:gs pos="0">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="65000"/>
-              <a:lumOff val="35000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="100000">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="85000"/>
-              <a:lumOff val="15000"/>
-            </a:schemeClr>
-          </a:gs>
-        </a:gsLst>
-        <a:path path="circle">
-          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-        </a:path>
-        <a:tileRect/>
-      </a:gradFill>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="34925" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="3">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:prstDash val="dash"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="10000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="5000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:prstDash val="dash"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="95000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
-      <a:effectLst>
-        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-          <a:prstClr val="black">
-            <a:alpha val="40000"/>
-          </a:prstClr>
-        </a:outerShdw>
-      </a:effectLst>
-    </cs:defRPr>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3626,7 +579,7 @@
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A10" sqref="A10:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
@@ -4211,8 +1164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C361"/>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="R3" sqref="L3:R3"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A286" workbookViewId="0">
+      <selection activeCell="F290" sqref="F290"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8193,7 +5146,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -8201,32 +5153,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
+    <sheetView rightToLeft="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="8.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
@@ -8245,7 +5197,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B3" s="1">
         <v>687</v>
@@ -8259,7 +5211,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B4" s="1">
         <v>672</v>
@@ -8273,7 +5225,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B5" s="1">
         <v>646</v>
@@ -8287,7 +5239,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B6" s="1">
         <v>613</v>
@@ -8301,7 +5253,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B7" s="1">
         <v>568</v>
@@ -8315,7 +5267,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B8" s="1">
         <v>500</v>
@@ -8329,7 +5281,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B9" s="1">
         <v>541</v>
@@ -8343,7 +5295,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B10" s="1">
         <v>571</v>
@@ -8357,7 +5309,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B11" s="1">
         <v>560</v>
@@ -8371,7 +5323,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B12" s="1">
         <v>558</v>
@@ -8385,7 +5337,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B13" s="1">
         <v>537</v>
@@ -8399,7 +5351,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B14" s="1">
         <v>539</v>
@@ -8413,7 +5365,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B15" s="1">
         <v>607</v>
@@ -8427,7 +5379,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B16" s="1">
         <v>597</v>
@@ -8441,7 +5393,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B17" s="1">
         <v>577</v>
@@ -8455,7 +5407,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B18" s="1">
         <v>624</v>
@@ -8469,7 +5421,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B19" s="1">
         <v>703</v>
@@ -8483,7 +5435,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B20" s="1">
         <v>695</v>
@@ -8497,7 +5449,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B21" s="1">
         <v>687</v>
@@ -8511,7 +5463,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B22" s="1">
         <v>684</v>
@@ -8525,7 +5477,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B23" s="1">
         <v>654</v>
@@ -8539,7 +5491,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B24" s="1">
         <v>638</v>
@@ -8553,7 +5505,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B25" s="1">
         <v>637</v>
@@ -8567,7 +5519,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B26" s="1">
         <v>627</v>

</xml_diff>